<commit_message>
[+] linq2sql, more new 64 bit hardware
</commit_message>
<xml_diff>
--- a/_results/RawResults.xlsx
+++ b/_results/RawResults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEXEY\DOCUMENTS\PROGRMG\VS2013\OrmTestNorthwind\_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTS\PROGRMG\VS2012\OrmTestNorthwind\_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>simple CF/10</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Without context</t>
   </si>
   <si>
-    <t>C2D E4700, DDR800, Win 8.1, 32 bit</t>
-  </si>
-  <si>
     <t>s CF/10+10</t>
   </si>
   <si>
@@ -138,6 +135,24 @@
   </si>
   <si>
     <t>s BLT/10+10</t>
+  </si>
+  <si>
+    <t>simple L2S/10</t>
+  </si>
+  <si>
+    <t>simple L2S/500</t>
+  </si>
+  <si>
+    <t>complex L2S/10</t>
+  </si>
+  <si>
+    <t>complex L2S/500</t>
+  </si>
+  <si>
+    <t>s L2S/10+10</t>
+  </si>
+  <si>
+    <t>i5-4200H, DDR3-1600, Win 8.1, 64 bit, .NET 4.5, EF 6.1.2</t>
   </si>
 </sst>
 </file>
@@ -471,11 +486,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I33"/>
+  <dimension ref="B1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -486,7 +499,7 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -522,29 +535,29 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1449</v>
+        <v>710</v>
       </c>
       <c r="D5">
-        <v>1447</v>
+        <v>721</v>
       </c>
       <c r="E5">
-        <v>1453</v>
+        <v>723</v>
       </c>
       <c r="F5" s="1">
         <f>(C5+D5+E5)/3</f>
-        <v>1449.6666666666667</v>
+        <v>718</v>
       </c>
       <c r="G5">
         <f>F5/1000</f>
-        <v>1.4496666666666667</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="H5" s="2">
-        <f>$H$29</f>
-        <v>0.2849999999999997</v>
+        <f>$H$33</f>
+        <v>0.17166666666666663</v>
       </c>
       <c r="I5">
         <f>G5-H5</f>
-        <v>1.164666666666667</v>
+        <v>0.54633333333333334</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -552,29 +565,29 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>3617</v>
+        <v>1814</v>
       </c>
       <c r="D6">
-        <v>3637</v>
+        <v>1857</v>
       </c>
       <c r="E6">
-        <v>3572</v>
+        <v>1853</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F33" si="0">(C6+D6+E6)/3</f>
-        <v>3608.6666666666665</v>
+        <f t="shared" ref="F6:F38" si="0">(C6+D6+E6)/3</f>
+        <v>1841.3333333333333</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G33" si="1">F6/1000</f>
-        <v>3.6086666666666667</v>
+        <f t="shared" ref="G6:G38" si="1">F6/1000</f>
+        <v>1.8413333333333333</v>
       </c>
       <c r="H6" s="2">
-        <f>$H$29</f>
-        <v>0.2849999999999997</v>
+        <f>$H$33</f>
+        <v>0.17166666666666663</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I28" si="2">G6-H6</f>
-        <v>3.323666666666667</v>
+        <f t="shared" ref="I6:I32" si="2">G6-H6</f>
+        <v>1.6696666666666666</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -582,29 +595,29 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>1507</v>
+        <v>748</v>
       </c>
       <c r="D7">
-        <v>1503</v>
+        <v>756</v>
       </c>
       <c r="E7">
-        <v>1496</v>
+        <v>747</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>1502</v>
+        <v>750.33333333333337</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>1.502</v>
+        <v>0.75033333333333341</v>
       </c>
       <c r="H7" s="2">
-        <f>$H$30</f>
-        <v>0.34533333333333349</v>
+        <f>$H$34</f>
+        <v>0.21199999999999997</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>1.1566666666666665</v>
+        <v>0.53833333333333344</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -612,29 +625,29 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>3649</v>
+        <v>1884</v>
       </c>
       <c r="D8">
-        <v>3650</v>
+        <v>1929</v>
       </c>
       <c r="E8">
-        <v>3633</v>
+        <v>1902</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>3644</v>
+        <v>1905</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>3.6440000000000001</v>
+        <v>1.905</v>
       </c>
       <c r="H8" s="2">
-        <f>$H$30</f>
-        <v>0.34533333333333349</v>
+        <f>$H$34</f>
+        <v>0.21199999999999997</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>3.2986666666666666</v>
+        <v>1.6930000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -642,29 +655,29 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>1603</v>
+        <v>849</v>
       </c>
       <c r="D9">
-        <v>1611</v>
+        <v>858</v>
       </c>
       <c r="E9">
-        <v>1604</v>
+        <v>827</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>1606</v>
+        <v>844.66666666666663</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>1.6060000000000001</v>
+        <v>0.84466666666666668</v>
       </c>
       <c r="H9" s="2">
-        <f>$H$31</f>
-        <v>0.64900000000000002</v>
+        <f>$H$35</f>
+        <v>0.37600000000000011</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>0.95700000000000007</v>
+        <v>0.46866666666666656</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -672,29 +685,29 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>3746</v>
+        <v>2076</v>
       </c>
       <c r="D10">
-        <v>3725</v>
+        <v>2121</v>
       </c>
       <c r="E10">
-        <v>3720</v>
+        <v>2047</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>3730.3333333333335</v>
+        <v>2081.3333333333335</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>3.7303333333333333</v>
+        <v>2.0813333333333337</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ref="H10:H12" si="3">$H$31</f>
-        <v>0.64900000000000002</v>
+        <f t="shared" ref="H10:H12" si="3">$H$35</f>
+        <v>0.37600000000000011</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>3.0813333333333333</v>
+        <v>1.7053333333333336</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -702,29 +715,29 @@
         <v>24</v>
       </c>
       <c r="C11">
-        <v>853</v>
+        <v>436</v>
       </c>
       <c r="D11">
-        <v>915</v>
+        <v>432</v>
       </c>
       <c r="E11">
-        <v>855</v>
+        <v>420</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>874.33333333333337</v>
+        <v>429.33333333333331</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>0.87433333333333341</v>
+        <v>0.42933333333333329</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="3"/>
-        <v>0.64900000000000002</v>
+        <v>0.37600000000000011</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>0.22533333333333339</v>
+        <v>5.3333333333333177E-2</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -732,615 +745,761 @@
         <v>25</v>
       </c>
       <c r="C12">
-        <v>3021</v>
+        <v>1538</v>
       </c>
       <c r="D12">
-        <v>3031</v>
+        <v>1612</v>
       </c>
       <c r="E12">
-        <v>3021</v>
+        <v>1550</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>3024.3333333333335</v>
+        <v>1566.6666666666667</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>3.0243333333333333</v>
+        <v>1.5666666666666667</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="3"/>
-        <v>0.64900000000000002</v>
+        <v>0.37600000000000011</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>2.3753333333333333</v>
+        <v>1.1906666666666665</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C13">
-        <v>277</v>
+        <v>938</v>
       </c>
       <c r="D13">
-        <v>309</v>
+        <v>1017</v>
       </c>
       <c r="E13">
-        <v>284</v>
+        <v>923</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>959.33333333333337</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
+        <v>0.95933333333333337</v>
       </c>
       <c r="H13" s="2">
-        <f>$H$32</f>
-        <v>8.4666666666666668E-2</v>
+        <f>$H$36</f>
+        <v>9.2666666666666675E-2</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>0.20533333333333331</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>2264</v>
+        <v>2031</v>
       </c>
       <c r="D14">
-        <v>2278</v>
+        <v>1939</v>
       </c>
       <c r="E14">
-        <v>2271</v>
+        <v>2009</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>2271</v>
+        <v>1993</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>2.2709999999999999</v>
+        <v>1.9930000000000001</v>
       </c>
       <c r="H14" s="2">
-        <f>$H$32</f>
-        <v>8.4666666666666668E-2</v>
+        <f>$H$36</f>
+        <v>9.2666666666666675E-2</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>2.1863333333333332</v>
+        <v>1.9003333333333334</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>347</v>
+        <v>127</v>
       </c>
       <c r="D15">
-        <v>338</v>
+        <v>127</v>
       </c>
       <c r="E15">
-        <v>339</v>
+        <v>126</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>341.33333333333331</v>
+        <v>126.66666666666667</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>0.34133333333333332</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="H15" s="2">
-        <f>$H$33</f>
-        <v>9.8999999999999977E-2</v>
+        <f>$H$37</f>
+        <v>3.3333333333333354E-2</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>0.24233333333333335</v>
+        <v>9.3333333333333324E-2</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>2537</v>
+        <v>980</v>
       </c>
       <c r="D16">
-        <v>2441</v>
+        <v>970</v>
       </c>
       <c r="E16">
-        <v>2476</v>
+        <v>968</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>2484.6666666666665</v>
+        <v>972.66666666666663</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>2.4846666666666666</v>
+        <v>0.97266666666666668</v>
       </c>
       <c r="H16" s="2">
-        <f>$H$33</f>
-        <v>9.8999999999999977E-2</v>
+        <f>$H$37</f>
+        <v>3.3333333333333354E-2</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>2.3856666666666664</v>
+        <v>0.93933333333333335</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>22674</v>
+        <v>156</v>
       </c>
       <c r="D17">
-        <v>22638</v>
+        <v>155</v>
       </c>
       <c r="E17">
-        <v>22679</v>
+        <v>156</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>22663.666666666668</v>
+        <v>155.66666666666666</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>22.663666666666668</v>
+        <v>0.15566666666666665</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17:H18" si="4">$H$29</f>
-        <v>0.2849999999999997</v>
+        <f>$H$38</f>
+        <v>4.433333333333328E-2</v>
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>22.378666666666668</v>
+        <v>0.11133333333333337</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>28042</v>
+        <v>1283</v>
       </c>
       <c r="D18">
-        <v>27742</v>
+        <v>1237</v>
       </c>
       <c r="E18">
-        <v>27786</v>
+        <v>1263</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>27856.666666666668</v>
+        <v>1261</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>27.856666666666669</v>
+        <v>1.2609999999999999</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="4"/>
-        <v>0.2849999999999997</v>
+        <f>$H$38</f>
+        <v>4.433333333333328E-2</v>
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>27.571666666666669</v>
+        <v>1.2166666666666666</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>22712</v>
+        <v>10831</v>
       </c>
       <c r="D19">
-        <v>22710</v>
+        <v>10604</v>
       </c>
       <c r="E19">
-        <v>22750</v>
+        <v>10629</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>22724</v>
+        <v>10688</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>22.724</v>
+        <v>10.688000000000001</v>
       </c>
       <c r="H19" s="2">
-        <f>$H$30</f>
-        <v>0.34533333333333349</v>
+        <f t="shared" ref="H19:H20" si="4">$H$33</f>
+        <v>0.17166666666666663</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>22.378666666666668</v>
+        <v>10.516333333333334</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>27846</v>
+        <v>13235</v>
       </c>
       <c r="D20">
-        <v>27752</v>
+        <v>13123</v>
       </c>
       <c r="E20">
-        <v>27852</v>
+        <v>13062</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>27816.666666666668</v>
+        <v>13140</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>27.816666666666666</v>
+        <v>13.14</v>
       </c>
       <c r="H20" s="2">
-        <f>$H$30</f>
-        <v>0.34533333333333349</v>
+        <f t="shared" si="4"/>
+        <v>0.17166666666666663</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>27.471333333333334</v>
+        <v>12.968333333333334</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>25404</v>
+        <v>10878</v>
       </c>
       <c r="D21">
-        <v>25425</v>
+        <v>10796</v>
       </c>
       <c r="E21">
-        <v>25396</v>
+        <v>10649</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>25408.333333333332</v>
+        <v>10774.333333333334</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>25.408333333333331</v>
+        <v>10.774333333333335</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ref="H21:H22" si="5">$H$31</f>
-        <v>0.64900000000000002</v>
+        <f>$H$34</f>
+        <v>0.21199999999999997</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>24.759333333333331</v>
+        <v>10.562333333333335</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>30489</v>
+        <v>13404</v>
       </c>
       <c r="D22">
-        <v>30545</v>
+        <v>13174</v>
       </c>
       <c r="E22">
-        <v>30601</v>
+        <v>13105</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>30545</v>
+        <v>13227.666666666666</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>30.545000000000002</v>
+        <v>13.227666666666666</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="5"/>
-        <v>0.64900000000000002</v>
+        <f>$H$34</f>
+        <v>0.21199999999999997</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>29.896000000000001</v>
+        <v>13.015666666666666</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>12603</v>
+      </c>
+      <c r="D23">
+        <v>12645</v>
+      </c>
+      <c r="E23">
+        <v>12434</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12560.666666666666</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="2"/>
+        <v>12.560666666666666</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" ref="H23:H24" si="5">$H$35</f>
+        <v>0.37600000000000011</v>
+      </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.184666666666667</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>15015</v>
+      </c>
+      <c r="D24">
+        <v>15086</v>
+      </c>
+      <c r="E24">
+        <v>14926</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15009</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="2"/>
+        <v>15.009</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="5"/>
+        <v>0.37600000000000011</v>
+      </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14.633000000000001</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>13627</v>
-      </c>
-      <c r="D25">
-        <v>13603</v>
-      </c>
-      <c r="E25">
-        <v>13584</v>
+        <v>26</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>13604.666666666666</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>13.604666666666667</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" ref="H25:H26" si="6">$H$32</f>
-        <v>8.4666666666666668E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2"/>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>13.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26">
-        <v>18258</v>
-      </c>
-      <c r="D26">
-        <v>18367</v>
-      </c>
-      <c r="E26">
-        <v>18210</v>
+        <v>27</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>18278.333333333332</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>18.278333333333332</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="6"/>
-        <v>8.4666666666666668E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H26" s="2"/>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>18.193666666666665</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C27">
-        <v>13693</v>
+        <v>9065</v>
       </c>
       <c r="D27">
-        <v>13654</v>
+        <v>9001</v>
       </c>
       <c r="E27">
-        <v>13632</v>
+        <v>8777</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>13659.666666666666</v>
+        <v>8947.6666666666661</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>13.659666666666666</v>
+        <v>8.9476666666666667</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ref="H27:H28" si="7">$H$33</f>
-        <v>9.8999999999999977E-2</v>
+        <f t="shared" ref="H27:H28" si="6">$H$36</f>
+        <v>9.2666666666666675E-2</v>
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>13.560666666666666</v>
+        <v>8.8550000000000004</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C28">
-        <v>18694</v>
+        <v>11402</v>
       </c>
       <c r="D28">
-        <v>18665</v>
+        <v>11189</v>
       </c>
       <c r="E28">
-        <v>18665</v>
+        <v>11233</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>18674.666666666668</v>
+        <v>11274.666666666666</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>18.674666666666667</v>
+        <v>11.274666666666667</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="7"/>
-        <v>9.8999999999999977E-2</v>
+        <f t="shared" si="6"/>
+        <v>9.2666666666666675E-2</v>
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>18.575666666666667</v>
+        <v>11.182</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>2607</v>
+        <v>4097</v>
       </c>
       <c r="D29">
-        <v>2631</v>
+        <v>4201</v>
       </c>
       <c r="E29">
-        <v>2605</v>
+        <v>4110</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>2614.3333333333335</v>
+        <v>4136</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>2.6143333333333336</v>
-      </c>
-      <c r="H29" s="3">
-        <f>2*G5-G29</f>
-        <v>0.2849999999999997</v>
+        <v>4.1360000000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" ref="H29:H30" si="7">$H$37</f>
+        <v>3.3333333333333354E-2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>4.1026666666666669</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>2666</v>
+        <v>6682</v>
       </c>
       <c r="D30">
-        <v>2670</v>
+        <v>6720</v>
       </c>
       <c r="E30">
-        <v>2640</v>
+        <v>6670</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>2658.6666666666665</v>
+        <v>6690.666666666667</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>2.6586666666666665</v>
-      </c>
-      <c r="H30" s="3">
-        <f>2*G7-G30</f>
-        <v>0.34533333333333349</v>
+        <v>6.690666666666667</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333354E-2</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>6.6573333333333338</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>2565</v>
+        <v>4143</v>
       </c>
       <c r="D31">
-        <v>2543</v>
+        <v>4193</v>
       </c>
       <c r="E31">
-        <v>2581</v>
+        <v>4134</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>2563</v>
+        <v>4156.666666666667</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>2.5630000000000002</v>
-      </c>
-      <c r="H31" s="3">
-        <f>2*G9-G31</f>
-        <v>0.64900000000000002</v>
+        <v>4.1566666666666672</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" ref="H31:H32" si="8">$H$38</f>
+        <v>4.433333333333328E-2</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>4.1123333333333338</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>503</v>
+        <v>7023</v>
       </c>
       <c r="D32">
-        <v>480</v>
+        <v>7062</v>
       </c>
       <c r="E32">
-        <v>503</v>
+        <v>6984</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>495.33333333333331</v>
+        <v>7023</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>0.49533333333333329</v>
-      </c>
-      <c r="H32" s="3">
-        <f>2*G13-G32</f>
-        <v>8.4666666666666668E-2</v>
+        <v>7.0229999999999997</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="8"/>
+        <v>4.433333333333328E-2</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>6.9786666666666664</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C33">
-        <v>582</v>
+        <v>1266</v>
       </c>
       <c r="D33">
-        <v>580</v>
+        <v>1258</v>
       </c>
       <c r="E33">
-        <v>589</v>
+        <v>1269</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
-        <v>583.66666666666663</v>
+        <v>1264.3333333333333</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>0.58366666666666667</v>
+        <v>1.2643333333333333</v>
       </c>
       <c r="H33" s="3">
-        <f>2*G15-G33</f>
-        <v>9.8999999999999977E-2</v>
+        <f>2*G5-G33</f>
+        <v>0.17166666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>1289</v>
+      </c>
+      <c r="D34">
+        <v>1292</v>
+      </c>
+      <c r="E34">
+        <v>1285</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>1288.6666666666667</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>1.2886666666666668</v>
+      </c>
+      <c r="H34" s="3">
+        <f>2*G7-G34</f>
+        <v>0.21199999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>1304</v>
+      </c>
+      <c r="D35">
+        <v>1315</v>
+      </c>
+      <c r="E35">
+        <v>1321</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="0"/>
+        <v>1313.3333333333333</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>1.3133333333333332</v>
+      </c>
+      <c r="H35" s="3">
+        <f>2*G9-G35</f>
+        <v>0.37600000000000011</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <v>1851</v>
+      </c>
+      <c r="D36">
+        <v>1896</v>
+      </c>
+      <c r="E36">
+        <v>1731</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="0"/>
+        <v>1826</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>1.8260000000000001</v>
+      </c>
+      <c r="H36" s="3">
+        <f>2*G13-G36</f>
+        <v>9.2666666666666675E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>220</v>
+      </c>
+      <c r="D37">
+        <v>220</v>
+      </c>
+      <c r="E37">
+        <v>220</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="H37" s="3">
+        <f>2*G15-G37</f>
+        <v>3.3333333333333354E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>270</v>
+      </c>
+      <c r="D38">
+        <v>264</v>
+      </c>
+      <c r="E38">
+        <v>267</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
+        <v>267</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="H38" s="3">
+        <f>2*G17-G38</f>
+        <v>4.433333333333328E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>